<commit_message>
Added Historical Var as a second step
</commit_message>
<xml_diff>
--- a/VaR_Report.xlsx
+++ b/VaR_Report.xlsx
@@ -725,7 +725,7 @@
     </row>
     <row r="2">
       <c r="A2" s="2" t="n">
-        <v>2634548.61</v>
+        <v>1524154.456000008</v>
       </c>
     </row>
   </sheetData>
@@ -766,7 +766,7 @@
         </is>
       </c>
       <c r="B2" s="2" t="n">
-        <v>1135306.01</v>
+        <v>1364332.8</v>
       </c>
     </row>
     <row r="3">
@@ -776,7 +776,7 @@
         </is>
       </c>
       <c r="B3" s="2" t="n">
-        <v>2592398.31</v>
+        <v>1897405.728000013</v>
       </c>
     </row>
     <row r="4">
@@ -786,7 +786,7 @@
         </is>
       </c>
       <c r="B4" s="2" t="n">
-        <v>76728.08</v>
+        <v>107847.9999999999</v>
       </c>
     </row>
   </sheetData>
@@ -828,7 +828,7 @@
         </is>
       </c>
       <c r="B2" s="2" t="n">
-        <v>2630555.09</v>
+        <v>1490154.456000008</v>
       </c>
     </row>
     <row r="3">
@@ -838,7 +838,7 @@
         </is>
       </c>
       <c r="B3" s="2" t="n">
-        <v>76728.08</v>
+        <v>107847.9999999999</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Removal of many unused functions
</commit_message>
<xml_diff>
--- a/VaR_Report.xlsx
+++ b/VaR_Report.xlsx
@@ -725,7 +725,7 @@
     </row>
     <row r="2">
       <c r="A2" s="2" t="n">
-        <v>1524154.456000008</v>
+        <v>619970.5599999964</v>
       </c>
     </row>
   </sheetData>
@@ -766,7 +766,7 @@
         </is>
       </c>
       <c r="B2" s="2" t="n">
-        <v>1364332.8</v>
+        <v>374335.9999999985</v>
       </c>
     </row>
     <row r="3">
@@ -776,7 +776,7 @@
         </is>
       </c>
       <c r="B3" s="2" t="n">
-        <v>1897405.728000013</v>
+        <v>701141.5200000077</v>
       </c>
     </row>
     <row r="4">
@@ -786,7 +786,7 @@
         </is>
       </c>
       <c r="B4" s="2" t="n">
-        <v>107847.9999999999</v>
+        <v>25262</v>
       </c>
     </row>
   </sheetData>
@@ -828,7 +828,7 @@
         </is>
       </c>
       <c r="B2" s="2" t="n">
-        <v>1490154.456000008</v>
+        <v>616426.0000000001</v>
       </c>
     </row>
     <row r="3">
@@ -838,7 +838,7 @@
         </is>
       </c>
       <c r="B3" s="2" t="n">
-        <v>107847.9999999999</v>
+        <v>25262</v>
       </c>
     </row>
   </sheetData>

</xml_diff>